<commit_message>
CORRECTED SPREADSHEETS AND CORRESPONDING SCRIPTS
- Corrected column header name in spreadsheet providing the sheath
  height
- Corrected the names of spreadsheet files being referenced by the
  function that generates and loads the LUTs
</commit_message>
<xml_diff>
--- a/data/Couedel_PhysRevE_105_015210_fig08_sheathHeight.xlsx
+++ b/data/Couedel_PhysRevE_105_015210_fig08_sheathHeight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgeaugustomartinezortiz/Documents/Github/VDRIAD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D9F833-B5A9-F844-B050-B9DF683E4811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C977F0-BCEF-924A-8C1E-3C066976EC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1120" windowWidth="27240" windowHeight="15940" xr2:uid="{F886CF64-15DC-5F47-8D42-C7FB1C7E2A7D}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>z</t>
+    <t>z0</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>